<commit_message>
1 stage repair marks
</commit_message>
<xml_diff>
--- a/Check.xlsx
+++ b/Check.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="47">
   <si>
     <t>Группа проверок</t>
   </si>
@@ -36,57 +36,15 @@
     <t>Высокий</t>
   </si>
   <si>
-    <t>Проверка раздела новости</t>
-  </si>
-  <si>
     <t>Сортировка новостей</t>
   </si>
   <si>
-    <t>Создание новости</t>
-  </si>
-  <si>
     <t>Статус</t>
   </si>
   <si>
-    <t>Удаление новости</t>
-  </si>
-  <si>
-    <t>Редактирование новости</t>
-  </si>
-  <si>
-    <t>Проверка раздела тематических цитат</t>
-  </si>
-  <si>
-    <t>Проверка раздела "о приложении"</t>
-  </si>
-  <si>
-    <t>Проверка наличия цитат</t>
-  </si>
-  <si>
-    <t>Проверка наличия информации в разделе</t>
-  </si>
-  <si>
-    <t>Выход из приложения при нажатии кнопки  выхода</t>
-  </si>
-  <si>
-    <t>Переход в раздел цитат при нажатии кнопки</t>
-  </si>
-  <si>
     <t>Средний</t>
   </si>
   <si>
-    <t>Авторизация с корректными данными</t>
-  </si>
-  <si>
-    <t>Авторизация с некорректными данными</t>
-  </si>
-  <si>
-    <t>Проверка работы выпадающего меню</t>
-  </si>
-  <si>
-    <t>Проверка элементов панели навигации</t>
-  </si>
-  <si>
     <t>Фильтр новостей</t>
   </si>
   <si>
@@ -94,6 +52,114 @@
   </si>
   <si>
     <t>Не выполнено</t>
+  </si>
+  <si>
+    <t>Авторизация с незарегистрированными данными</t>
+  </si>
+  <si>
+    <t>Авторизация с зарегистрированными данными</t>
+  </si>
+  <si>
+    <t>Элементы панели навигации</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Раздел новости</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Раздел тематических цитат</t>
+  </si>
+  <si>
+    <t>Наличие цитат</t>
+  </si>
+  <si>
+    <t>Раздел "о приложении"</t>
+  </si>
+  <si>
+    <t>Наличие информации в разделе</t>
+  </si>
+  <si>
+    <t>Валидация поля ввода логин</t>
+  </si>
+  <si>
+    <t>Валидация поля ввода пароль</t>
+  </si>
+  <si>
+    <t>Пустая форма отправки</t>
+  </si>
+  <si>
+    <t>Чтение новости</t>
+  </si>
+  <si>
+    <t>Переход в режим редактирования новостей</t>
+  </si>
+  <si>
+    <t>Чтение цитат</t>
+  </si>
+  <si>
+    <t>Переход в раздел новости</t>
+  </si>
+  <si>
+    <t>Переход в раздел "о приложении"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Переход в раздел цитат </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Выход из приложения </t>
+  </si>
+  <si>
+    <t>Работа выпадающего меню</t>
+  </si>
+  <si>
+    <t>Смена ориентации экрана</t>
+  </si>
+  <si>
+    <t>Восстановление после сворачивания приложения</t>
+  </si>
+  <si>
+    <t>Работа при входящем вызове</t>
+  </si>
+  <si>
+    <t>Работа при сети 3G</t>
+  </si>
+  <si>
+    <t>Работа при сети 2G</t>
+  </si>
+  <si>
+    <t>Работа при Wi-Fi</t>
+  </si>
+  <si>
+    <t>Работа при отсутствии сети</t>
+  </si>
+  <si>
+    <t>Работа при входящих SMS</t>
+  </si>
+  <si>
+    <t>Воздействия со стороны Android</t>
+  </si>
+  <si>
+    <t>Локализация приложения (смена языка ОС)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Удаление новости</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Редактирование новости</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Сортировка новостей</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Фильтр Новостей</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Создание новости</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Чтение новости</t>
+  </si>
+  <si>
+    <t>Ссылки</t>
   </si>
 </sst>
 </file>
@@ -117,7 +183,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -175,10 +241,34 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -188,35 +278,45 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -498,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -513,188 +613,435 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="10"/>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="10"/>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="10"/>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="13"/>
+      <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="13"/>
+      <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="13"/>
+      <c r="B10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="14"/>
+      <c r="B11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="13"/>
+      <c r="B13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="13"/>
+      <c r="B14" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="C14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="13"/>
+      <c r="B15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="13"/>
+      <c r="B16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="13"/>
+      <c r="B17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="13"/>
+      <c r="B18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="13"/>
+      <c r="B19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="13"/>
+      <c r="B20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="14"/>
+      <c r="B21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="11"/>
+      <c r="B23" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="1" t="s">
+      <c r="C24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="11"/>
+      <c r="B25" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="10"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>24</v>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="10"/>
+      <c r="B27" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="10"/>
+      <c r="B28" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="10"/>
+      <c r="B29" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="10"/>
+      <c r="B30" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="10"/>
+      <c r="B31" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="10"/>
+      <c r="B32" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="10"/>
+      <c r="B33" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="11"/>
+      <c r="B34" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
+  <mergeCells count="6">
+    <mergeCell ref="A26:A34"/>
     <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A12:A21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>